<commit_message>
deleted Done todos work with archive file FIX
</commit_message>
<xml_diff>
--- a/files/archived_tasks.xlsx
+++ b/files/archived_tasks.xlsx
@@ -1,229 +1,192 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14580" windowHeight="11070" activeTab="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="14580" windowHeight="11070" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-08-17" sheetId="1" r:id="rId1"/>
-    <sheet name="2024-08-18" sheetId="2" r:id="rId2"/>
+    <sheet name="2024-08-17" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2024-08-18" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2024-08-19" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
-  <si>
-    <t>Archived Tasks</t>
-  </si>
-  <si>
-    <t>Eat</t>
-  </si>
-  <si>
-    <t>Shit</t>
-  </si>
-  <si>
-    <t>Sleep</t>
-  </si>
-  <si>
-    <t>Repeat</t>
-  </si>
-  <si>
-    <t>Do Some Of The Python Cours</t>
-  </si>
-  <si>
-    <t>Upgrade This App</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
+  <fonts count="22">
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <b val="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <b val="1"/>
+      <color theme="3"/>
       <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <b val="1"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="33">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -415,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -536,157 +499,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -742,11 +714,74 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1033,85 +1068,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Archived Tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Eat</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Shit</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sleep</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Repeat</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Archived Tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Eat</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Do Some Of The Python Cours</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Shit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Upgrade This App</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Archived Tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Today 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>All Day</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix + removal of useless code
</commit_message>
<xml_diff>
--- a/files/archived_tasks.xlsx
+++ b/files/archived_tasks.xlsx
@@ -1181,7 +1181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1217,6 +1217,13 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Today 5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>